<commit_message>
add interface for reference and school
</commit_message>
<xml_diff>
--- a/docment/webapi doc/api.xlsx
+++ b/docment/webapi doc/api.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
   <si>
     <t>URL/地址</t>
   </si>
@@ -114,6 +114,18 @@
     <t>上传学校数据</t>
   </si>
   <si>
+    <t>host:port/api/School/GetById</t>
+  </si>
+  <si>
+    <t>id(int)</t>
+  </si>
+  <si>
+    <t>{"Id":"主键","Name":"学校名称","ShortName":"学校简称","AreaId":"所属区域id","AreaName":"区域名称"}</t>
+  </si>
+  <si>
+    <t>根据id获取学校信息，包含区域信息</t>
+  </si>
+  <si>
     <t>host:port/api/School/Update</t>
   </si>
   <si>
@@ -160,6 +172,24 @@
   </si>
   <si>
     <t>上传推荐人数据</t>
+  </si>
+  <si>
+    <t>host:port/api/References/GetBySchoolName</t>
+  </si>
+  <si>
+    <t>sch_name(string)</t>
+  </si>
+  <si>
+    <t>根据大学名称模糊查询推荐人消息</t>
+  </si>
+  <si>
+    <t>host:port/api/References/GetById</t>
+  </si>
+  <si>
+    <t>{"Id":"主键","Name":"推荐人姓名","Tel":"推荐人电话","SchoolId":"所属学校id","SchoolName":"学校名称"}</t>
+  </si>
+  <si>
+    <t>根据推荐人id获取信息，包含学校信息</t>
   </si>
   <si>
     <t>host=192.168.1.8 port:8899</t>
@@ -170,12 +200,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,9 +236,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -235,31 +265,64 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -280,75 +343,35 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,187 +386,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,24 +571,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -590,17 +589,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -616,6 +618,32 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -638,19 +666,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -659,152 +676,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -812,9 +829,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1167,17 +1181,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="34.325" style="1" customWidth="1"/>
+    <col min="1" max="1" width="45.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="52.625" style="1" customWidth="1"/>
@@ -1211,28 +1225,28 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="3"/>
       <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1241,19 +1255,19 @@
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1262,19 +1276,19 @@
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1283,13 +1297,13 @@
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -1297,7 +1311,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1306,7 +1320,7 @@
       <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1317,7 +1331,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1326,7 +1340,7 @@
       <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1337,131 +1351,191 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>36</v>
+      <c r="E10" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>42</v>
+      <c r="E12" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="G14" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
del references and school data feature and fix bug for export order data by condition
</commit_message>
<xml_diff>
--- a/docment/webapi doc/api.xlsx
+++ b/docment/webapi doc/api.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80">
   <si>
     <t>URL/地址</t>
   </si>
@@ -225,7 +225,37 @@
     <t>根据学校id分页获取，FullName满足学校+人名</t>
   </si>
   <si>
-    <t>host=192.168.1.8 port:8899</t>
+    <t>host:port/api/References/Del</t>
+  </si>
+  <si>
+    <t>id=1</t>
+  </si>
+  <si>
+    <t>根据id删除推荐人数据</t>
+  </si>
+  <si>
+    <t>host:port/api/References/DelRange</t>
+  </si>
+  <si>
+    <t>ids(int,int,int)</t>
+  </si>
+  <si>
+    <t>ids=1,1,1</t>
+  </si>
+  <si>
+    <t>根据ids批量删除推荐人数据</t>
+  </si>
+  <si>
+    <t>host:port/api/School/Del</t>
+  </si>
+  <si>
+    <t>根据id删除学校数据，删除给出警告，这样会连同相关推荐人一起删除</t>
+  </si>
+  <si>
+    <t>host:port/api/School/DelRange</t>
+  </si>
+  <si>
+    <t>根据ids批量删除学校数据，删除给出警告，这样会连同相关推荐人一起删除</t>
   </si>
 </sst>
 </file>
@@ -233,10 +263,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -260,76 +290,91 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -351,56 +396,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -419,181 +449,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -618,6 +648,54 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -629,15 +707,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -661,45 +730,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -712,10 +742,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -724,133 +754,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1214,12 +1244,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="6"/>
@@ -1602,7 +1632,6 @@
       <c r="E20" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
         <v>64</v>
       </c>
@@ -1623,14 +1652,88 @@
       <c r="E21" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:7">
+      <c r="A23" s="1" t="s">
         <v>69</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>